<commit_message>
update 31R in direct N2O reference injection
</commit_message>
<xml_diff>
--- a/pyisotopomer_examples/00_Python_template_v3.xlsx
+++ b/pyisotopomer_examples/00_Python_template_v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/N2O Research/N2O_isotopocule_data_corrections/pyisotopomer/pyisotopomer_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA915F1-A313-7D44-A1EC-F76AF0806275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54DC44D9-2C03-8D4B-9BD0-8ADCE9E435D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37980" yWindow="-5500" windowWidth="37860" windowHeight="23500" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="Rsolve18">_xlfn.LAMBDA(_xlpm.Rsam18,_xlpm.n,_xlpm.Rsam45,_xlpm.Rsam46,_xlpm.D17O,_xlpm.k,_xlpm.RVSMOW18,_xlpm.RVSMOW17,       IF(_xlpm.n&gt;0,Rsolve18(_xlfn.LET(_xlpm.Rsam17,(1 + _xlpm.D17O / 1000) * _xlpm.RVSMOW17 * (_xlpm.Rsam18/_xlpm.RVSMOW18) ^ _xlpm.k,         _xlpm.Rsam46 - (_xlpm.Rsam45 - _xlpm.Rsam17) * _xlpm.Rsam17 - (_xlpm.Rsam45 - _xlpm.Rsam17) ^ 2/4),_xlpm.n-1,_xlpm.Rsam45,_xlpm.Rsam46,_xlpm.D17O,_xlpm.k,_xlpm.RVSMOW18,_xlpm.RVSMOW17),               _xlpm.Rsam18))</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3987,8 +3987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357C812C-3217-554B-B2A1-EA8A97EA775D}">
   <dimension ref="A1:BM54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4318,7 +4318,7 @@
         <v>0.42840719999999999</v>
       </c>
       <c r="W3" s="25">
-        <v>3.73376282567055E-3</v>
+        <v>3.7347517422551104E-3</v>
       </c>
       <c r="X3" s="26">
         <v>7.7410249496226297E-3</v>
@@ -4361,7 +4361,7 @@
       <c r="AK3" s="32"/>
       <c r="AL3" s="33">
         <f>AE3*$W$3</f>
-        <v>3.7690253636311292E-3</v>
+        <v>3.7700236197774754E-3</v>
       </c>
       <c r="AM3" s="33">
         <f>AI3*$X$3</f>
@@ -4547,7 +4547,7 @@
       <c r="AK4" s="32"/>
       <c r="AL4" s="33">
         <f t="shared" ref="AL4:AL17" si="7">AE4*$W$3</f>
-        <v>3.7382429851740414E-3</v>
+        <v>3.7392330883642441E-3</v>
       </c>
       <c r="AM4" s="33">
         <f t="shared" ref="AM4:AM17" si="8">AI4*$X$3</f>
@@ -4738,7 +4738,7 @@
       <c r="AK5" s="32"/>
       <c r="AL5" s="33">
         <f t="shared" si="7"/>
-        <v>3.7228017752489757E-3</v>
+        <v>3.7237877887127293E-3</v>
       </c>
       <c r="AM5" s="33">
         <f t="shared" si="8"/>
@@ -4933,7 +4933,7 @@
       <c r="AK6" s="32"/>
       <c r="AL6" s="33">
         <f t="shared" si="7"/>
-        <v>3.7689117349450109E-3</v>
+        <v>3.7699099609959015E-3</v>
       </c>
       <c r="AM6" s="33">
         <f t="shared" si="8"/>
@@ -5128,7 +5128,7 @@
       <c r="AK7" s="32"/>
       <c r="AL7" s="33">
         <f t="shared" si="7"/>
-        <v>3.7376533142238627E-3</v>
+        <v>3.7386432612350551E-3</v>
       </c>
       <c r="AM7" s="33">
         <f t="shared" si="8"/>
@@ -5314,7 +5314,7 @@
       <c r="AK8" s="32"/>
       <c r="AL8" s="33">
         <f t="shared" si="7"/>
-        <v>3.7199285353648262E-3</v>
+        <v>3.7209137878282954E-3</v>
       </c>
       <c r="AM8" s="33">
         <f t="shared" si="8"/>
@@ -5504,7 +5504,7 @@
       </c>
       <c r="AL9" s="33">
         <f t="shared" si="7"/>
-        <v>3.770760540076305E-3</v>
+        <v>3.7717592557978421E-3</v>
       </c>
       <c r="AM9" s="33">
         <f t="shared" si="8"/>
@@ -5693,7 +5693,7 @@
       </c>
       <c r="AL10" s="33">
         <f t="shared" si="7"/>
-        <v>3.7559237220544848E-3</v>
+        <v>3.7569185081275437E-3</v>
       </c>
       <c r="AM10" s="33">
         <f t="shared" si="8"/>
@@ -5888,7 +5888,7 @@
       </c>
       <c r="AL11" s="33">
         <f t="shared" si="7"/>
-        <v>3.7741574091857285E-3</v>
+        <v>3.7751570245948877E-3</v>
       </c>
       <c r="AM11" s="33">
         <f t="shared" si="8"/>
@@ -6083,7 +6083,7 @@
       </c>
       <c r="AL12" s="33">
         <f t="shared" si="7"/>
-        <v>3.7381947000342886E-3</v>
+        <v>3.7391847904357902E-3</v>
       </c>
       <c r="AM12" s="33">
         <f t="shared" si="8"/>
@@ -6267,7 +6267,7 @@
       </c>
       <c r="AL13" s="33">
         <f t="shared" si="7"/>
-        <v>3.7242631653031056E-3</v>
+        <v>3.7252495658275614E-3</v>
       </c>
       <c r="AM13" s="33">
         <f t="shared" si="8"/>
@@ -6451,7 +6451,7 @@
       </c>
       <c r="AL14" s="33">
         <f t="shared" si="7"/>
-        <v>3.7661587198913019E-3</v>
+        <v>3.767156216784404E-3</v>
       </c>
       <c r="AM14" s="33">
         <f t="shared" si="8"/>
@@ -6635,7 +6635,7 @@
       </c>
       <c r="AL15" s="33">
         <f t="shared" si="7"/>
-        <v>3.7730126315774341E-3</v>
+        <v>3.7740119437831986E-3</v>
       </c>
       <c r="AM15" s="33">
         <f t="shared" si="8"/>
@@ -6819,7 +6819,7 @@
       </c>
       <c r="AL16" s="33">
         <f t="shared" si="7"/>
-        <v>3.7385509216503769E-3</v>
+        <v>3.7395411063999877E-3</v>
       </c>
       <c r="AM16" s="33">
         <f t="shared" si="8"/>
@@ -6999,7 +6999,7 @@
       </c>
       <c r="AL17" s="33">
         <f t="shared" si="7"/>
-        <v>3.7557778240511282E-3</v>
+        <v>3.7567725714819484E-3</v>
       </c>
       <c r="AM17" s="33">
         <f t="shared" si="8"/>

</xml_diff>

<commit_message>
solve for 18R first in calculate_17R.py
</commit_message>
<xml_diff>
--- a/pyisotopomer_examples/00_Python_template_v3.xlsx
+++ b/pyisotopomer_examples/00_Python_template_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/N2O Research/N2O_isotopocule_data_corrections/pyisotopomer/pyisotopomer_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54DC44D9-2C03-8D4B-9BD0-8ADCE9E435D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716B17A4-E4FB-2747-BE7C-E34528479DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37980" yWindow="-5500" windowWidth="37860" windowHeight="23500" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
   </bookViews>
   <sheets>
     <sheet name="size_correction" sheetId="2" r:id="rId1"/>
@@ -775,22 +775,26 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="19">
@@ -3987,8 +3991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357C812C-3217-554B-B2A1-EA8A97EA775D}">
   <dimension ref="A1:BM54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AI4" sqref="AI4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8036,8 +8040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131672C0-DA0C-0746-8A59-3EFE5C746DAE}">
   <dimension ref="A1:AA47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Z5" sqref="Z5"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="Y4" sqref="Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
update README with preprint link
</commit_message>
<xml_diff>
--- a/pyisotopomer_examples/00_Python_template_v3.xlsx
+++ b/pyisotopomer_examples/00_Python_template_v3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/N2O Research/N2O_isotopocule_data_corrections/pyisotopomer/pyisotopomer_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/PhD Research/N2O_isotopocule_data_corrections/pyisotopomer/pyisotopomer_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41518C93-58AF-D648-99DC-20C256437315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799CCE28-49A8-5B4E-8B69-5F48647616DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12960" yWindow="500" windowWidth="15840" windowHeight="15880" activeTab="1" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{C87639FE-6F05-2348-B25E-B6AD821683A8}"/>
   </bookViews>
   <sheets>
     <sheet name="size_correction" sheetId="2" r:id="rId1"/>
@@ -800,6 +800,7 @@
       <sz val="12"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="19">
@@ -1169,7 +1170,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1387,6 +1388,7 @@
     <xf numFmtId="2" fontId="0" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="25" fillId="16" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1399,7 +1401,12 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="25" fillId="16" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -1586,49 +1593,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>5.6690060748599133E-3</c:v>
+                  <c:v>5.6690055237280769E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-3.3157633670658081E-3</c:v>
+                  <c:v>-3.3157638681124957E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.8320385549917295E-4</c:v>
+                  <c:v>3.8320389860548991E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.3855513126554056E-3</c:v>
+                  <c:v>6.3855507699817496E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-3.3736683280273967E-3</c:v>
+                  <c:v>-3.3736677173379051E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-8.2966123175853173E-4</c:v>
+                  <c:v>-8.2966119409939951E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.0812199816469847E-3</c:v>
+                  <c:v>5.0812194379027328E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-9.1141789753790732E-3</c:v>
+                  <c:v>-9.1141790851831522E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.7029884167436144E-3</c:v>
+                  <c:v>5.7029878614330018E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-3.5945739634335372E-3</c:v>
+                  <c:v>-3.5945744132340751E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.7966870305363727E-4</c:v>
+                  <c:v>1.7966872284646754E-4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.8686826228146419E-3</c:v>
+                  <c:v>4.8686820742108883E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.6228928832132777E-3</c:v>
+                  <c:v>5.622892326012742E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-3.6734640658408848E-3</c:v>
+                  <c:v>-3.6734644937986794E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-6.5263177824188435E-3</c:v>
+                  <c:v>-6.5263180168436035E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2118,49 +2125,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>7.4936919644022753E-3</c:v>
+                  <c:v>7.4936924442244243E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-5.0356547842637621E-3</c:v>
+                  <c:v>-5.0356543464973921E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.3013837783483656E-3</c:v>
+                  <c:v>4.3013837408978879E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.6776086292741075E-3</c:v>
+                  <c:v>7.6776091019842571E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-4.8488753146248009E-3</c:v>
+                  <c:v>-4.8488758480560003E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.3832486035312902E-3</c:v>
+                  <c:v>2.3832485707903322E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.6953639452707308E-3</c:v>
+                  <c:v>5.695364419234337E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.9256582960658154E-3</c:v>
+                  <c:v>4.9256583905018169E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.4477259185061388E-3</c:v>
+                  <c:v>5.4477264029729328E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-6.2381121983366193E-3</c:v>
+                  <c:v>-6.2381118049810447E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.0262381999534996E-3</c:v>
+                  <c:v>4.0262381827564685E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.3456591947391319E-3</c:v>
+                  <c:v>5.3456596730043536E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.446829485110093E-3</c:v>
+                  <c:v>6.4468299707013997E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-5.2698268942697113E-3</c:v>
+                  <c:v>-5.2698265204076363E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.3905400058642007E-3</c:v>
+                  <c:v>4.3905402081100102E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3990,8 +3997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357C812C-3217-554B-B2A1-EA8A97EA775D}">
   <dimension ref="A1:BM54"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3:Y3"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="W19" sqref="W19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4341,36 +4348,36 @@
       </c>
       <c r="AE3" s="31">
         <f>$W$7*(20-I3)+AC3</f>
-        <v>1.0094442361786187</v>
+        <v>1.0094442359432119</v>
       </c>
       <c r="AF3" s="31">
         <f>$X$7*(20-I3)+AA3</f>
-        <v>1.0056851052976181</v>
+        <v>1.005685104743353</v>
       </c>
       <c r="AG3" s="31">
         <f>$Y$7*(20-I3)+AB3</f>
-        <v>1.0075218399408568</v>
+        <v>1.0075218404242881</v>
       </c>
       <c r="AI3" s="68">
         <f>AF3^$X$11*EXP(X$12)</f>
-        <v>1.0058729966944395</v>
+        <v>1.0058729965987645</v>
       </c>
       <c r="AJ3" s="68">
         <f>AG3^$Y$11*EXP(Y$12)</f>
-        <v>1.0044845842983396</v>
+        <v>1.004484584452265</v>
       </c>
       <c r="AK3" s="32"/>
       <c r="AL3" s="33">
         <f>AE3*$W$3</f>
-        <v>3.7690253636311274E-3</v>
+        <v>3.7690253627521743E-3</v>
       </c>
       <c r="AM3" s="33">
         <f>AI3*$X$3</f>
-        <v>7.7864879635633402E-3</v>
+        <v>7.7864879628227173E-3</v>
       </c>
       <c r="AN3" s="33">
         <f>AJ3*$Y$3</f>
-        <v>2.1107186571324705E-3</v>
+        <v>2.1107186574559132E-3</v>
       </c>
       <c r="AO3" s="112">
         <v>0</v>
@@ -4526,36 +4533,36 @@
       </c>
       <c r="AE4" s="31">
         <f t="shared" ref="AE4:AE17" si="2">$W$7*(20-I4)+AC4</f>
-        <v>1.0011999046840065</v>
+        <v>1.0011999044719069</v>
       </c>
       <c r="AF4" s="31">
         <f t="shared" ref="AF4:AF17" si="3">$X$7*(20-I4)+AA4</f>
-        <v>0.99668972770557829</v>
+        <v>0.9966897272061902</v>
       </c>
       <c r="AG4" s="31">
         <f t="shared" ref="AG4:AG17" si="4">$Y$7*(20-I4)+AB4</f>
-        <v>0.99497700286985102</v>
+        <v>0.99497700330541849</v>
       </c>
       <c r="AI4" s="68">
         <f t="shared" ref="AI4:AI17" si="5">AF4^$X$11*EXP(X$12)</f>
-        <v>0.99767868588737729</v>
+        <v>0.99767868558186468</v>
       </c>
       <c r="AJ4" s="68">
         <f t="shared" ref="AJ4:AJ17" si="6">AG4^$Y$11*EXP(Y$12)</f>
-        <v>0.99357291603893838</v>
+        <v>0.99357291625992428</v>
       </c>
       <c r="AK4" s="32"/>
       <c r="AL4" s="33">
         <f t="shared" ref="AL4:AL17" si="7">AE4*$W$3</f>
-        <v>3.7382429851740397E-3</v>
+        <v>3.7382429843821098E-3</v>
       </c>
       <c r="AM4" s="33">
         <f t="shared" ref="AM4:AM17" si="8">AI4*$X$3</f>
-        <v>7.7230555991609088E-3</v>
+        <v>7.7230555967959282E-3</v>
       </c>
       <c r="AN4" s="33">
         <f t="shared" ref="AN4:AN17" si="9">AJ4*$Y$3</f>
-        <v>2.0877900207595724E-3</v>
+        <v>2.0877900212239288E-3</v>
       </c>
       <c r="AO4" s="112">
         <v>0</v>
@@ -4716,36 +4723,36 @@
       </c>
       <c r="AE5" s="31">
         <f t="shared" si="2"/>
-        <v>0.99706434207705574</v>
+        <v>0.99706434209537076</v>
       </c>
       <c r="AF5" s="31">
         <f t="shared" si="3"/>
-        <v>1.0003832772874761</v>
+        <v>1.000383277330599</v>
       </c>
       <c r="AG5" s="31">
         <f t="shared" si="4"/>
-        <v>1.0043106480077921</v>
+        <v>1.0043106479701802</v>
       </c>
       <c r="AI5" s="68">
         <f t="shared" si="5"/>
-        <v>1.001044111578594</v>
+        <v>1.0010441118737647</v>
       </c>
       <c r="AJ5" s="68">
         <f t="shared" si="6"/>
-        <v>1.001693114134492</v>
+        <v>1.0016931138633087</v>
       </c>
       <c r="AK5" s="32"/>
       <c r="AL5" s="33">
         <f t="shared" si="7"/>
-        <v>3.7228017752489739E-3</v>
+        <v>3.7228017753173576E-3</v>
       </c>
       <c r="AM5" s="33">
         <f t="shared" si="8"/>
-        <v>7.7491074434027181E-3</v>
+        <v>7.749107445687642E-3</v>
       </c>
       <c r="AN5" s="33">
         <f t="shared" si="9"/>
-        <v>2.1048529542160065E-3</v>
+        <v>2.1048529536461702E-3</v>
       </c>
       <c r="AO5" s="112">
         <v>0</v>
@@ -4890,7 +4897,7 @@
       <c r="W6" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="X6" s="16" t="s">
+      <c r="X6" s="124" t="s">
         <v>20</v>
       </c>
       <c r="Y6" s="17" t="s">
@@ -4910,36 +4917,36 @@
       </c>
       <c r="AE6" s="31">
         <f t="shared" si="2"/>
-        <v>1.0094138034244713</v>
+        <v>1.0094138031925111</v>
       </c>
       <c r="AF6" s="31">
         <f t="shared" si="3"/>
-        <v>1.0064059824102283</v>
+        <v>1.0064059818640783</v>
       </c>
       <c r="AG6" s="31">
         <f t="shared" si="4"/>
-        <v>1.0077071570383731</v>
+        <v>1.0077071575147265</v>
       </c>
       <c r="AI6" s="68">
         <f t="shared" si="5"/>
-        <v>1.0065293924891645</v>
+        <v>1.0065293924217837</v>
       </c>
       <c r="AJ6" s="68">
         <f t="shared" si="6"/>
-        <v>1.0046456444970819</v>
+        <v>1.0046456446432428</v>
       </c>
       <c r="AK6" s="32"/>
       <c r="AL6" s="33">
         <f t="shared" si="7"/>
-        <v>3.7689117349450092E-3</v>
+        <v>3.7689117340789246E-3</v>
       </c>
       <c r="AM6" s="33">
         <f t="shared" si="8"/>
-        <v>7.7915691397871332E-3</v>
+        <v>7.7915691392655374E-3</v>
       </c>
       <c r="AN6" s="33">
         <f t="shared" si="9"/>
-        <v>2.1110570921584735E-3</v>
+        <v>2.1110570924656007E-3</v>
       </c>
       <c r="AO6" s="112">
         <v>0</v>
@@ -5081,14 +5088,14 @@
       <c r="U7" s="24">
         <v>0.42891970000000001</v>
       </c>
-      <c r="W7" s="34">
-        <v>5.65785154557688E-5</v>
-      </c>
-      <c r="X7" s="35">
-        <v>2.8107236390596598E-5</v>
-      </c>
-      <c r="Y7" s="36">
-        <v>4.8711468260038703E-5</v>
+      <c r="W7" s="125">
+        <v>5.65785E-5</v>
+      </c>
+      <c r="X7" s="126">
+        <v>2.8107200000000001E-5</v>
+      </c>
+      <c r="Y7" s="127">
+        <v>4.8711500000000003E-5</v>
       </c>
       <c r="AA7" s="28">
         <f t="shared" si="1"/>
@@ -5104,36 +5111,36 @@
       </c>
       <c r="AE7" s="31">
         <f t="shared" si="2"/>
-        <v>1.0010419752766739</v>
+        <v>1.0010419755351716</v>
       </c>
       <c r="AF7" s="31">
         <f t="shared" si="3"/>
-        <v>0.99663201609671503</v>
+        <v>0.99663201670534773</v>
       </c>
       <c r="AG7" s="31">
         <f t="shared" si="4"/>
-        <v>0.9951628615034982</v>
+        <v>0.99516286097264728</v>
       </c>
       <c r="AI7" s="68">
         <f t="shared" si="5"/>
-        <v>0.99762609234989208</v>
+        <v>0.99762609305247885</v>
       </c>
       <c r="AJ7" s="68">
         <f t="shared" si="6"/>
-        <v>0.99373470664282637</v>
+        <v>0.99373470602094893</v>
       </c>
       <c r="AK7" s="32"/>
       <c r="AL7" s="33">
         <f t="shared" si="7"/>
-        <v>3.737653314223861E-3</v>
+        <v>3.7376533151890303E-3</v>
       </c>
       <c r="AM7" s="33">
         <f t="shared" si="8"/>
-        <v>7.7226484712750471E-3</v>
+        <v>7.7226484767137886E-3</v>
       </c>
       <c r="AN7" s="33">
         <f t="shared" si="9"/>
-        <v>2.0881299905824179E-3</v>
+        <v>2.0881299892756698E-3</v>
       </c>
       <c r="AO7" s="112">
         <v>0</v>
@@ -5289,36 +5296,36 @@
       </c>
       <c r="AE8" s="31">
         <f t="shared" si="2"/>
-        <v>0.99629481277958798</v>
+        <v>0.9962948127955692</v>
       </c>
       <c r="AF8" s="31">
         <f t="shared" si="3"/>
-        <v>0.99917068284195976</v>
+        <v>0.99917068287958766</v>
       </c>
       <c r="AG8" s="31">
         <f t="shared" si="4"/>
-        <v>1.0023860907979212</v>
+        <v>1.0023860907651021</v>
       </c>
       <c r="AI8" s="68">
         <f t="shared" si="5"/>
-        <v>0.99993936333439959</v>
+        <v>0.99993936358963498</v>
       </c>
       <c r="AJ8" s="68">
         <f t="shared" si="6"/>
-        <v>1.0000195594494503</v>
+        <v>1.0000195591990293</v>
       </c>
       <c r="AK8" s="32"/>
       <c r="AL8" s="33">
         <f t="shared" si="7"/>
-        <v>3.7199285353648245E-3</v>
+        <v>3.7199285354244942E-3</v>
       </c>
       <c r="AM8" s="33">
         <f t="shared" si="8"/>
-        <v>7.7405555596813573E-3</v>
+        <v>7.7405555616571415E-3</v>
       </c>
       <c r="AN8" s="33">
         <f t="shared" si="9"/>
-        <v>2.101336321753283E-3</v>
+        <v>2.1013363212270745E-3</v>
       </c>
       <c r="AO8" s="112">
         <v>0</v>
@@ -5479,35 +5486,35 @@
       </c>
       <c r="AE9" s="31">
         <f t="shared" si="2"/>
-        <v>1.0099089621203003</v>
+        <v>1.0099089618881856</v>
       </c>
       <c r="AF9" s="31">
         <f t="shared" si="3"/>
-        <v>1.0050941512728657</v>
+        <v>1.0050941507263516</v>
       </c>
       <c r="AG9" s="31">
         <f t="shared" si="4"/>
-        <v>1.0057116133646442</v>
+        <v>1.0057116138413149</v>
       </c>
       <c r="AI9" s="68">
         <f t="shared" si="5"/>
-        <v>1.0053348711319792</v>
+        <v>1.0053348710262333</v>
       </c>
       <c r="AJ9" s="68">
         <f t="shared" si="6"/>
-        <v>1.0029111055919546</v>
+        <v>1.0029111057557523</v>
       </c>
       <c r="AL9" s="33">
         <f t="shared" si="7"/>
-        <v>3.7707605400763033E-3</v>
+        <v>3.770760539209642E-3</v>
       </c>
       <c r="AM9" s="33">
         <f t="shared" si="8"/>
-        <v>7.7823223201583048E-3</v>
+        <v>7.7823223193397234E-3</v>
       </c>
       <c r="AN9" s="33">
         <f t="shared" si="9"/>
-        <v>2.1074123138454925E-3</v>
+        <v>2.1074123141896798E-3</v>
       </c>
       <c r="AO9" s="112">
         <v>0</v>
@@ -5668,35 +5675,35 @@
       </c>
       <c r="AE10" s="31">
         <f t="shared" si="2"/>
-        <v>1.0059352715795371</v>
+        <v>1.0059352715333243</v>
       </c>
       <c r="AF10" s="31">
         <f t="shared" si="3"/>
-        <v>0.99092722925764687</v>
+        <v>0.99092722914883902</v>
       </c>
       <c r="AG10" s="31">
         <f t="shared" si="4"/>
-        <v>1.0049378092932522</v>
+        <v>1.0049378093881545</v>
       </c>
       <c r="AI10" s="68">
         <f t="shared" si="5"/>
-        <v>0.99242587706510954</v>
+        <v>0.99242587695028661</v>
       </c>
       <c r="AJ10" s="68">
         <f t="shared" si="6"/>
-        <v>1.0022383915761395</v>
+        <v>1.0022383914147521</v>
       </c>
       <c r="AL10" s="33">
         <f t="shared" si="7"/>
-        <v>3.755923722054483E-3</v>
+        <v>3.7559237218819353E-3</v>
       </c>
       <c r="AM10" s="33">
         <f t="shared" si="8"/>
-        <v>7.6823934750121364E-3</v>
+        <v>7.6823934741232893E-3</v>
       </c>
       <c r="AN10" s="33">
         <f t="shared" si="9"/>
-        <v>2.1059987430985735E-3</v>
+        <v>2.1059987427594507E-3</v>
       </c>
       <c r="AO10" s="112">
         <v>0</v>
@@ -5843,11 +5850,11 @@
       </c>
       <c r="X11">
         <f>scale_normalization!Y3</f>
-        <v>0.91041071995587675</v>
+        <v>0.91041074852700155</v>
       </c>
       <c r="Y11" s="118">
         <f>scale_normalization!Z3</f>
-        <v>0.87174417962681128</v>
+        <v>0.87174417117952785</v>
       </c>
       <c r="AA11" s="28">
         <f t="shared" si="1"/>
@@ -5863,35 +5870,35 @@
       </c>
       <c r="AE11" s="31">
         <f t="shared" si="2"/>
-        <v>1.0108187331121987</v>
+        <v>1.0108187328749989</v>
       </c>
       <c r="AF11" s="31">
         <f t="shared" si="3"/>
-        <v>1.0057192814133826</v>
+        <v>1.005719280854896</v>
       </c>
       <c r="AG11" s="31">
         <f t="shared" si="4"/>
-        <v>1.0054625917600983</v>
+        <v>1.0054625922472116</v>
       </c>
       <c r="AI11" s="68">
         <f t="shared" si="5"/>
-        <v>1.005904116762288</v>
+        <v>1.0059041166637595</v>
       </c>
       <c r="AJ11" s="68">
         <f t="shared" si="6"/>
-        <v>1.0026946235102945</v>
+        <v>1.0026946236853349</v>
       </c>
       <c r="AL11" s="33">
         <f t="shared" si="7"/>
-        <v>3.7741574091857267E-3</v>
+        <v>3.7741574083000788E-3</v>
       </c>
       <c r="AM11" s="33">
         <f t="shared" si="8"/>
-        <v>7.786728864784989E-3</v>
+        <v>7.786728864022277E-3</v>
       </c>
       <c r="AN11" s="33">
         <f t="shared" si="9"/>
-        <v>2.1069574210817433E-3</v>
+        <v>2.106957421449555E-3</v>
       </c>
       <c r="AO11" s="112">
         <v>0</v>
@@ -6038,11 +6045,11 @@
       </c>
       <c r="X12" s="35">
         <f>scale_normalization!Y4</f>
-        <v>6.9469397524750496E-4</v>
+        <v>6.9469421991735661E-4</v>
       </c>
       <c r="Y12" s="36">
         <f>scale_normalization!Z4</f>
-        <v>-2.0580238405652936E-3</v>
+        <v>-2.0580240423078121E-3</v>
       </c>
       <c r="AA12" s="28">
         <f t="shared" si="1"/>
@@ -6058,35 +6065,35 @@
       </c>
       <c r="AE12" s="31">
         <f t="shared" si="2"/>
-        <v>1.0011869726521643</v>
+        <v>1.0011869724618112</v>
       </c>
       <c r="AF12" s="31">
         <f t="shared" si="3"/>
-        <v>0.99641187878361481</v>
+        <v>0.99641187833542821</v>
       </c>
       <c r="AG12" s="31">
         <f t="shared" si="4"/>
-        <v>0.99378130442821833</v>
+        <v>0.99378130481912774</v>
       </c>
       <c r="AI12" s="68">
         <f t="shared" si="5"/>
-        <v>0.99742547509365276</v>
+        <v>0.9974254748268071</v>
       </c>
       <c r="AJ12" s="68">
         <f t="shared" si="6"/>
-        <v>0.99253196355980511</v>
+        <v>0.99253196375221542</v>
       </c>
       <c r="AL12" s="33">
         <f t="shared" si="7"/>
-        <v>3.7381947000342869E-3</v>
+        <v>3.7381946993235537E-3</v>
       </c>
       <c r="AM12" s="33">
         <f t="shared" si="8"/>
-        <v>7.7210954880891731E-3</v>
+        <v>7.7210954860235147E-3</v>
       </c>
       <c r="AN12" s="33">
         <f t="shared" si="9"/>
-        <v>2.0856026722892822E-3</v>
+        <v>2.0856026726935933E-3</v>
       </c>
       <c r="AO12" s="112">
         <v>0</v>
@@ -6242,35 +6249,35 @@
       </c>
       <c r="AE13" s="31">
         <f t="shared" si="2"/>
-        <v>0.99745574081403032</v>
+        <v>0.99745574082243826</v>
       </c>
       <c r="AF13" s="31">
         <f t="shared" si="3"/>
-        <v>1.0001796848444418</v>
+        <v>1.0001796848642381</v>
       </c>
       <c r="AG13" s="31">
         <f t="shared" si="4"/>
-        <v>1.0040343543858852</v>
+        <v>1.0040343543686188</v>
       </c>
       <c r="AI13" s="68">
         <f t="shared" si="5"/>
-        <v>1.000858634704451</v>
+        <v>1.0008586349725039</v>
       </c>
       <c r="AJ13" s="68">
         <f t="shared" si="6"/>
-        <v>1.0014528802854337</v>
+        <v>1.0014528800343248</v>
       </c>
       <c r="AL13" s="33">
         <f t="shared" si="7"/>
-        <v>3.7242631653031039E-3</v>
+        <v>3.7242631653344972E-3</v>
       </c>
       <c r="AM13" s="33">
         <f t="shared" si="8"/>
-        <v>7.7476716622923991E-3</v>
+        <v>7.7476716643674034E-3</v>
       </c>
       <c r="AN13" s="33">
         <f t="shared" si="9"/>
-        <v>2.1043481519769196E-3</v>
+        <v>2.1043481514492657E-3</v>
       </c>
       <c r="AO13" s="112">
         <v>0</v>
@@ -6426,35 +6433,35 @@
       </c>
       <c r="AE14" s="31">
         <f t="shared" si="2"/>
-        <v>1.0086764735022862</v>
+        <v>1.0086764732681468</v>
       </c>
       <c r="AF14" s="31">
         <f t="shared" si="3"/>
-        <v>1.0048805539160894</v>
+        <v>1.0048805533648082</v>
       </c>
       <c r="AG14" s="31">
         <f t="shared" si="4"/>
-        <v>1.0053599727245706</v>
+        <v>1.0053599732053993</v>
       </c>
       <c r="AI14" s="68">
         <f t="shared" si="5"/>
-        <v>1.0051403613834002</v>
+        <v>1.0051403612671246</v>
       </c>
       <c r="AJ14" s="68">
         <f t="shared" si="6"/>
-        <v>1.0026054116498198</v>
+        <v>1.0026054118202889</v>
       </c>
       <c r="AL14" s="33">
         <f t="shared" si="7"/>
-        <v>3.7661587198913001E-3</v>
+        <v>3.7661587190170789E-3</v>
       </c>
       <c r="AM14" s="33">
         <f t="shared" si="8"/>
-        <v>7.7808166153416104E-3</v>
+        <v>7.7808166144415171E-3</v>
       </c>
       <c r="AN14" s="33">
         <f t="shared" si="9"/>
-        <v>2.1067699606256199E-3</v>
+        <v>2.106769960983826E-3</v>
       </c>
       <c r="AO14" s="112">
         <v>0</v>
@@ -6610,35 +6617,35 @@
       </c>
       <c r="AE15" s="31">
         <f t="shared" si="2"/>
-        <v>1.0105121315250749</v>
+        <v>1.0105121312870871</v>
       </c>
       <c r="AF15" s="31">
         <f t="shared" si="3"/>
-        <v>1.0056387310168626</v>
+        <v>1.0056387304565202</v>
       </c>
       <c r="AG15" s="31">
         <f t="shared" si="4"/>
-        <v>1.0064676550191509</v>
+        <v>1.0064676555078829</v>
       </c>
       <c r="AI15" s="68">
         <f t="shared" si="5"/>
-        <v>1.0058307690770196</v>
+        <v>1.0058307689744661</v>
       </c>
       <c r="AJ15" s="68">
         <f t="shared" si="6"/>
-        <v>1.0035683135664484</v>
+        <v>1.0035683137341556</v>
       </c>
       <c r="AL15" s="33">
         <f t="shared" si="7"/>
-        <v>3.7730126315774323E-3</v>
+        <v>3.7730126306888424E-3</v>
       </c>
       <c r="AM15" s="33">
         <f t="shared" si="8"/>
-        <v>7.7861610785233291E-3</v>
+        <v>7.7861610777294598E-3</v>
       </c>
       <c r="AN15" s="33">
         <f t="shared" si="9"/>
-        <v>2.1087933018218777E-3</v>
+        <v>2.1087933021742803E-3</v>
       </c>
       <c r="AO15" s="112">
         <v>0</v>
@@ -6794,35 +6801,35 @@
       </c>
       <c r="AE16" s="31">
         <f t="shared" si="2"/>
-        <v>1.0012823781807745</v>
+        <v>1.0012823779996793</v>
       </c>
       <c r="AF16" s="31">
         <f t="shared" si="3"/>
-        <v>0.99633327484903467</v>
+        <v>0.99633327442264608</v>
       </c>
       <c r="AG16" s="31">
         <f t="shared" si="4"/>
-        <v>0.99474403428411884</v>
+        <v>0.99474403465601591</v>
       </c>
       <c r="AI16" s="68">
         <f t="shared" si="5"/>
-        <v>0.99735384017979356</v>
+        <v>0.99735383993055227</v>
       </c>
       <c r="AJ16" s="68">
         <f t="shared" si="6"/>
-        <v>0.99337011057906566</v>
+        <v>0.99337011074663262</v>
       </c>
       <c r="AL16" s="33">
         <f t="shared" si="7"/>
-        <v>3.7385509216503751E-3</v>
+        <v>3.7385509209742086E-3</v>
       </c>
       <c r="AM16" s="33">
         <f t="shared" si="8"/>
-        <v>7.7205409604337253E-3</v>
+        <v>7.7205409585043424E-3</v>
       </c>
       <c r="AN16" s="33">
         <f t="shared" si="9"/>
-        <v>2.0873638666158321E-3</v>
+        <v>2.0873638669679398E-3</v>
       </c>
       <c r="AO16" s="112">
         <v>0</v>
@@ -6974,35 +6981,35 @@
       </c>
       <c r="AE17" s="31">
         <f t="shared" si="2"/>
-        <v>1.0058961962525363</v>
+        <v>1.0058961961536195</v>
       </c>
       <c r="AF17" s="31">
         <f t="shared" si="3"/>
-        <v>0.99349493237592013</v>
+        <v>0.99349493214302032</v>
       </c>
       <c r="AG17" s="31">
         <f t="shared" si="4"/>
-        <v>1.0044001925480899</v>
+        <v>1.0044001927512256</v>
       </c>
       <c r="AI17" s="68">
         <f t="shared" si="5"/>
-        <v>0.9947668054279567</v>
+        <v>0.99476680527355188</v>
       </c>
       <c r="AJ17" s="68">
         <f t="shared" si="6"/>
-        <v>1.001770970173647</v>
+        <v>1.0017709701110122</v>
       </c>
       <c r="AL17" s="33">
         <f t="shared" si="7"/>
-        <v>3.7557778240511265E-3</v>
+        <v>3.7557778236817943E-3</v>
       </c>
       <c r="AM17" s="33">
         <f t="shared" si="8"/>
-        <v>7.7005146598742155E-3</v>
+        <v>7.7005146586789641E-3</v>
       </c>
       <c r="AN17" s="33">
         <f t="shared" si="9"/>
-        <v>2.1050165527390537E-3</v>
+        <v>2.1050165526074398E-3</v>
       </c>
       <c r="AO17" s="112">
         <v>0</v>
@@ -7869,7 +7876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131672C0-DA0C-0746-8A59-3EFE5C746DAE}">
   <dimension ref="A1:AA47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -7896,24 +7903,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="120" t="s">
         <v>177</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119"/>
-      <c r="G1" s="120" t="s">
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="121" t="s">
         <v>115</v>
       </c>
-      <c r="H1" s="120"/>
-      <c r="I1" s="120"/>
-      <c r="J1" s="120"/>
-      <c r="K1" s="120"/>
-      <c r="L1" s="120"/>
-      <c r="M1" s="120"/>
-      <c r="N1" s="120"/>
+      <c r="H1" s="121"/>
+      <c r="I1" s="121"/>
+      <c r="J1" s="121"/>
+      <c r="K1" s="121"/>
+      <c r="L1" s="121"/>
+      <c r="M1" s="121"/>
+      <c r="N1" s="121"/>
       <c r="O1" s="105" t="s">
         <v>114</v>
       </c>
@@ -8072,19 +8079,19 @@
       </c>
       <c r="S3" s="102">
         <f>size_correction!AF3</f>
-        <v>1.0056851052976181</v>
+        <v>1.005685104743353</v>
       </c>
       <c r="T3" s="102">
         <f>size_correction!AG3</f>
-        <v>1.0075218399408568</v>
+        <v>1.0075218404242881</v>
       </c>
       <c r="U3" s="60">
         <f t="shared" ref="U3:U17" si="1">LN(S3)</f>
-        <v>5.6690060748599133E-3</v>
+        <v>5.6690055237280769E-3</v>
       </c>
       <c r="V3" s="60">
         <f t="shared" ref="V3:V17" si="2">LN(T3)</f>
-        <v>7.4936919644022753E-3</v>
+        <v>7.4936924442244243E-3</v>
       </c>
       <c r="W3" s="60">
         <f t="shared" ref="W3:X9" si="3">LN(Q3)</f>
@@ -8096,11 +8103,11 @@
       </c>
       <c r="Y3" s="64">
         <f>SLOPE(W3:W54,U3:U54)</f>
-        <v>0.91041071995587675</v>
+        <v>0.91041074852700155</v>
       </c>
       <c r="Z3" s="64">
         <f>SLOPE(X3:X54,V3:V54)</f>
-        <v>0.87174417962681128</v>
+        <v>0.87174417117952785</v>
       </c>
       <c r="AA3" t="s">
         <v>181</v>
@@ -8173,19 +8180,19 @@
       </c>
       <c r="S4" s="102">
         <f>size_correction!AF4</f>
-        <v>0.99668972770557829</v>
+        <v>0.9966897272061902</v>
       </c>
       <c r="T4" s="102">
         <f>size_correction!AG4</f>
-        <v>0.99497700286985102</v>
+        <v>0.99497700330541849</v>
       </c>
       <c r="U4" s="60">
         <f t="shared" si="1"/>
-        <v>-3.3157633670658081E-3</v>
+        <v>-3.3157638681124957E-3</v>
       </c>
       <c r="V4" s="60">
         <f t="shared" si="2"/>
-        <v>-5.0356547842637621E-3</v>
+        <v>-5.0356543464973921E-3</v>
       </c>
       <c r="W4" s="60">
         <f t="shared" si="3"/>
@@ -8197,11 +8204,11 @@
       </c>
       <c r="Y4" s="64">
         <f>INTERCEPT(W3:W54,U3:U54)</f>
-        <v>6.9469397524750496E-4</v>
+        <v>6.9469421991735661E-4</v>
       </c>
       <c r="Z4" s="64">
         <f>INTERCEPT(X3:X54,V3:V54)</f>
-        <v>-2.0580238405652936E-3</v>
+        <v>-2.0580240423078121E-3</v>
       </c>
       <c r="AA4" t="s">
         <v>182</v>
@@ -8274,19 +8281,19 @@
       </c>
       <c r="S5" s="102">
         <f>size_correction!AF5</f>
-        <v>1.0003832772874761</v>
+        <v>1.000383277330599</v>
       </c>
       <c r="T5" s="102">
         <f>size_correction!AG5</f>
-        <v>1.0043106480077921</v>
+        <v>1.0043106479701802</v>
       </c>
       <c r="U5" s="60">
         <f t="shared" si="1"/>
-        <v>3.8320385549917295E-4</v>
+        <v>3.8320389860548991E-4</v>
       </c>
       <c r="V5" s="60">
         <f t="shared" si="2"/>
-        <v>4.3013837783483656E-3</v>
+        <v>4.3013837408978879E-3</v>
       </c>
       <c r="W5" s="60">
         <f t="shared" si="3"/>
@@ -8364,19 +8371,19 @@
       </c>
       <c r="S6" s="102">
         <f>size_correction!AF6</f>
-        <v>1.0064059824102283</v>
+        <v>1.0064059818640783</v>
       </c>
       <c r="T6" s="102">
         <f>size_correction!AG6</f>
-        <v>1.0077071570383731</v>
+        <v>1.0077071575147265</v>
       </c>
       <c r="U6" s="60">
         <f t="shared" si="1"/>
-        <v>6.3855513126554056E-3</v>
+        <v>6.3855507699817496E-3</v>
       </c>
       <c r="V6" s="60">
         <f t="shared" si="2"/>
-        <v>7.6776086292741075E-3</v>
+        <v>7.6776091019842571E-3</v>
       </c>
       <c r="W6" s="60">
         <f t="shared" si="3"/>
@@ -8454,19 +8461,19 @@
       </c>
       <c r="S7" s="102">
         <f>size_correction!AF7</f>
-        <v>0.99663201609671503</v>
+        <v>0.99663201670534773</v>
       </c>
       <c r="T7" s="102">
         <f>size_correction!AG7</f>
-        <v>0.9951628615034982</v>
+        <v>0.99516286097264728</v>
       </c>
       <c r="U7" s="60">
         <f t="shared" si="1"/>
-        <v>-3.3736683280273967E-3</v>
+        <v>-3.3736677173379051E-3</v>
       </c>
       <c r="V7" s="60">
         <f t="shared" si="2"/>
-        <v>-4.8488753146248009E-3</v>
+        <v>-4.8488758480560003E-3</v>
       </c>
       <c r="W7" s="60">
         <f t="shared" si="3"/>
@@ -8544,19 +8551,19 @@
       </c>
       <c r="S8" s="102">
         <f>size_correction!AF8</f>
-        <v>0.99917068284195976</v>
+        <v>0.99917068287958766</v>
       </c>
       <c r="T8" s="102">
         <f>size_correction!AG8</f>
-        <v>1.0023860907979212</v>
+        <v>1.0023860907651021</v>
       </c>
       <c r="U8" s="60">
         <f t="shared" si="1"/>
-        <v>-8.2966123175853173E-4</v>
+        <v>-8.2966119409939951E-4</v>
       </c>
       <c r="V8" s="60">
         <f t="shared" si="2"/>
-        <v>2.3832486035312902E-3</v>
+        <v>2.3832485707903322E-3</v>
       </c>
       <c r="W8" s="60">
         <f t="shared" si="3"/>
@@ -8634,19 +8641,19 @@
       </c>
       <c r="S9" s="102">
         <f>size_correction!AF9</f>
-        <v>1.0050941512728657</v>
+        <v>1.0050941507263516</v>
       </c>
       <c r="T9" s="102">
         <f>size_correction!AG9</f>
-        <v>1.0057116133646442</v>
+        <v>1.0057116138413149</v>
       </c>
       <c r="U9" s="60">
         <f t="shared" si="1"/>
-        <v>5.0812199816469847E-3</v>
+        <v>5.0812194379027328E-3</v>
       </c>
       <c r="V9" s="60">
         <f t="shared" si="2"/>
-        <v>5.6953639452707308E-3</v>
+        <v>5.695364419234337E-3</v>
       </c>
       <c r="W9" s="60">
         <f t="shared" si="3"/>
@@ -8661,17 +8668,17 @@
       <c r="A10" s="108">
         <v>94321</v>
       </c>
-      <c r="B10" s="123">
+      <c r="B10" s="119">
         <v>50.52</v>
       </c>
-      <c r="C10" s="123">
+      <c r="C10" s="119">
         <v>2.21</v>
       </c>
       <c r="D10" s="109">
         <f t="shared" ref="D10" si="12">AVERAGE(B10:C10)</f>
         <v>26.365000000000002</v>
       </c>
-      <c r="E10" s="123">
+      <c r="E10" s="119">
         <v>35.54</v>
       </c>
       <c r="F10" s="109">
@@ -8724,19 +8731,19 @@
       </c>
       <c r="S10" s="102">
         <f>size_correction!AF10</f>
-        <v>0.99092722925764687</v>
+        <v>0.99092722914883902</v>
       </c>
       <c r="T10" s="102">
         <f>size_correction!AG10</f>
-        <v>1.0049378092932522</v>
+        <v>1.0049378093881545</v>
       </c>
       <c r="U10" s="60">
         <f t="shared" ref="U10" si="20">LN(S10)</f>
-        <v>-9.1141789753790732E-3</v>
+        <v>-9.1141790851831522E-3</v>
       </c>
       <c r="V10" s="60">
         <f t="shared" ref="V10" si="21">LN(T10)</f>
-        <v>4.9256582960658154E-3</v>
+        <v>4.9256583905018169E-3</v>
       </c>
       <c r="W10" s="60">
         <f t="shared" ref="W10" si="22">LN(Q10)</f>
@@ -8764,19 +8771,19 @@
       </c>
       <c r="S11" s="102">
         <f>size_correction!AF11</f>
-        <v>1.0057192814133826</v>
+        <v>1.005719280854896</v>
       </c>
       <c r="T11" s="102">
         <f>size_correction!AG11</f>
-        <v>1.0054625917600983</v>
+        <v>1.0054625922472116</v>
       </c>
       <c r="U11" s="60">
         <f t="shared" si="1"/>
-        <v>5.7029884167436144E-3</v>
+        <v>5.7029878614330018E-3</v>
       </c>
       <c r="V11" s="60">
         <f t="shared" si="2"/>
-        <v>5.4477259185061388E-3</v>
+        <v>5.4477264029729328E-3</v>
       </c>
       <c r="W11" s="60">
         <f t="shared" ref="W11:X16" si="25">LN(Q11)</f>
@@ -8804,19 +8811,19 @@
       </c>
       <c r="S12" s="102">
         <f>size_correction!AF12</f>
-        <v>0.99641187878361481</v>
+        <v>0.99641187833542821</v>
       </c>
       <c r="T12" s="102">
         <f>size_correction!AG12</f>
-        <v>0.99378130442821833</v>
+        <v>0.99378130481912774</v>
       </c>
       <c r="U12" s="60">
         <f t="shared" si="1"/>
-        <v>-3.5945739634335372E-3</v>
+        <v>-3.5945744132340751E-3</v>
       </c>
       <c r="V12" s="60">
         <f t="shared" si="2"/>
-        <v>-6.2381121983366193E-3</v>
+        <v>-6.2381118049810447E-3</v>
       </c>
       <c r="W12" s="60">
         <f t="shared" si="25"/>
@@ -8842,19 +8849,19 @@
       </c>
       <c r="S13" s="102">
         <f>size_correction!AF13</f>
-        <v>1.0001796848444418</v>
+        <v>1.0001796848642381</v>
       </c>
       <c r="T13" s="102">
         <f>size_correction!AG13</f>
-        <v>1.0040343543858852</v>
+        <v>1.0040343543686188</v>
       </c>
       <c r="U13" s="60">
         <f t="shared" si="1"/>
-        <v>1.7966870305363727E-4</v>
+        <v>1.7966872284646754E-4</v>
       </c>
       <c r="V13" s="60">
         <f t="shared" si="2"/>
-        <v>4.0262381999534996E-3</v>
+        <v>4.0262381827564685E-3</v>
       </c>
       <c r="W13" s="60">
         <f t="shared" si="25"/>
@@ -8880,19 +8887,19 @@
       </c>
       <c r="S14" s="102">
         <f>size_correction!AF14</f>
-        <v>1.0048805539160894</v>
+        <v>1.0048805533648082</v>
       </c>
       <c r="T14" s="102">
         <f>size_correction!AG14</f>
-        <v>1.0053599727245706</v>
+        <v>1.0053599732053993</v>
       </c>
       <c r="U14" s="60">
         <f t="shared" si="1"/>
-        <v>4.8686826228146419E-3</v>
+        <v>4.8686820742108883E-3</v>
       </c>
       <c r="V14" s="60">
         <f t="shared" si="2"/>
-        <v>5.3456591947391319E-3</v>
+        <v>5.3456596730043536E-3</v>
       </c>
       <c r="W14" s="60">
         <f t="shared" si="25"/>
@@ -8918,19 +8925,19 @@
       </c>
       <c r="S15" s="102">
         <f>size_correction!AF15</f>
-        <v>1.0056387310168626</v>
+        <v>1.0056387304565202</v>
       </c>
       <c r="T15" s="102">
         <f>size_correction!AG15</f>
-        <v>1.0064676550191509</v>
+        <v>1.0064676555078829</v>
       </c>
       <c r="U15" s="60">
         <f t="shared" si="1"/>
-        <v>5.6228928832132777E-3</v>
+        <v>5.622892326012742E-3</v>
       </c>
       <c r="V15" s="60">
         <f t="shared" si="2"/>
-        <v>6.446829485110093E-3</v>
+        <v>6.4468299707013997E-3</v>
       </c>
       <c r="W15" s="60">
         <f t="shared" si="25"/>
@@ -8956,19 +8963,19 @@
       </c>
       <c r="S16" s="102">
         <f>size_correction!AF16</f>
-        <v>0.99633327484903467</v>
+        <v>0.99633327442264608</v>
       </c>
       <c r="T16" s="102">
         <f>size_correction!AG16</f>
-        <v>0.99474403428411884</v>
+        <v>0.99474403465601591</v>
       </c>
       <c r="U16" s="60">
         <f t="shared" si="1"/>
-        <v>-3.6734640658408848E-3</v>
+        <v>-3.6734644937986794E-3</v>
       </c>
       <c r="V16" s="60">
         <f t="shared" si="2"/>
-        <v>-5.2698268942697113E-3</v>
+        <v>-5.2698265204076363E-3</v>
       </c>
       <c r="W16" s="60">
         <f t="shared" si="25"/>
@@ -8988,19 +8995,19 @@
       <c r="R17" s="61"/>
       <c r="S17" s="102">
         <f>size_correction!AF17</f>
-        <v>0.99349493237592013</v>
+        <v>0.99349493214302032</v>
       </c>
       <c r="T17" s="102">
         <f>size_correction!AG17</f>
-        <v>1.0044001925480899</v>
+        <v>1.0044001927512256</v>
       </c>
       <c r="U17" s="60">
         <f t="shared" si="1"/>
-        <v>-6.5263177824188435E-3</v>
+        <v>-6.5263180168436035E-3</v>
       </c>
       <c r="V17" s="60">
         <f t="shared" si="2"/>
-        <v>4.3905400058642007E-3</v>
+        <v>4.3905402081100102E-3</v>
       </c>
       <c r="W17" s="60"/>
       <c r="X17" s="60"/>
@@ -9145,22 +9152,22 @@
       <c r="S2" s="69"/>
     </row>
     <row r="3" spans="1:25">
-      <c r="A3" s="121" t="s">
+      <c r="A3" s="122" t="s">
         <v>171</v>
       </c>
-      <c r="B3" s="121"/>
-      <c r="C3" s="121"/>
-      <c r="D3" s="121"/>
-      <c r="E3" s="121"/>
-      <c r="F3" s="121"/>
-      <c r="G3" s="122" t="s">
+      <c r="B3" s="122"/>
+      <c r="C3" s="122"/>
+      <c r="D3" s="122"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="122"/>
+      <c r="G3" s="123" t="s">
         <v>172</v>
       </c>
-      <c r="H3" s="122"/>
-      <c r="I3" s="122"/>
-      <c r="J3" s="122"/>
-      <c r="K3" s="122"/>
-      <c r="L3" s="122"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="123"/>
+      <c r="J3" s="123"/>
+      <c r="K3" s="123"/>
+      <c r="L3" s="123"/>
       <c r="M3" t="s">
         <v>125</v>
       </c>

</xml_diff>